<commit_message>
cambios en las interfaces
</commit_message>
<xml_diff>
--- a/src/informesGenerados/CertificoHechos.xlsx
+++ b/src/informesGenerados/CertificoHechos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>U/O</t>
   </si>
@@ -37,76 +37,43 @@
     <t>Otros delitos</t>
   </si>
   <si>
-    <t>DTNO</t>
+    <t>DTLT</t>
+  </si>
+  <si>
+    <t>DTVC</t>
+  </si>
+  <si>
+    <t>DTSC</t>
+  </si>
+  <si>
+    <t>DTPR</t>
+  </si>
+  <si>
+    <t>DTMY</t>
+  </si>
+  <si>
+    <t>DTGR</t>
   </si>
   <si>
     <t>DVLS</t>
   </si>
   <si>
-    <t>DTMZ</t>
-  </si>
-  <si>
-    <t>DTSC</t>
-  </si>
-  <si>
-    <t>DTAR</t>
-  </si>
-  <si>
-    <t>DTSS</t>
-  </si>
-  <si>
-    <t>DTSR</t>
+    <t>DTES</t>
+  </si>
+  <si>
+    <t>DTGT</t>
+  </si>
+  <si>
+    <t>DTCF</t>
   </si>
   <si>
     <t>DTOE</t>
   </si>
   <si>
-    <t>DVTI</t>
-  </si>
-  <si>
-    <t>DTGT</t>
-  </si>
-  <si>
-    <t>DVSF</t>
-  </si>
-  <si>
-    <t>DTCA</t>
-  </si>
-  <si>
-    <t>DTVC</t>
-  </si>
-  <si>
-    <t>DTGR</t>
-  </si>
-  <si>
     <t>DTHO</t>
   </si>
   <si>
-    <t>DVPE</t>
-  </si>
-  <si>
-    <t>DTES</t>
-  </si>
-  <si>
-    <t>DTIJ</t>
-  </si>
-  <si>
     <t>DTCM</t>
-  </si>
-  <si>
-    <t>DTLT</t>
-  </si>
-  <si>
-    <t>DTMY</t>
-  </si>
-  <si>
-    <t>DTPR</t>
-  </si>
-  <si>
-    <t>DVLH</t>
-  </si>
-  <si>
-    <t>DTCF</t>
   </si>
 </sst>
 </file>
@@ -558,7 +525,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
   <sheetPr/>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScale="100" view="normal"/>
   </sheetViews>
@@ -592,13 +559,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E2" s="3">
         <v>0</v>
@@ -618,10 +585,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
@@ -630,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -638,16 +605,16 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
@@ -661,13 +628,13 @@
         <v>10</v>
       </c>
       <c r="B5" s="3">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
       </c>
       <c r="D5" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
@@ -684,13 +651,13 @@
         <v>11</v>
       </c>
       <c r="B6" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D6" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
@@ -707,13 +674,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -722,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -730,19 +697,19 @@
         <v>13</v>
       </c>
       <c r="B8" s="3">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
       </c>
       <c r="F8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -759,16 +726,16 @@
         <v>0</v>
       </c>
       <c r="D9" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3">
         <v>0</v>
       </c>
       <c r="G9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -776,7 +743,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -802,10 +769,10 @@
         <v>0</v>
       </c>
       <c r="C11" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
@@ -814,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -828,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
@@ -837,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -845,7 +812,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="3">
         <v>0</v>
@@ -864,279 +831,26 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="3">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3">
-        <v>2</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="3">
-        <v>7</v>
-      </c>
-      <c r="C15" s="3">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="3">
-        <v>8</v>
-      </c>
-      <c r="C16" s="3">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="3">
-        <v>0</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
-        <v>2</v>
-      </c>
-      <c r="E17" s="3">
-        <v>0</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="3">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3">
-        <v>4</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>0</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="3">
-        <v>0</v>
-      </c>
-      <c r="C19" s="3">
-        <v>2</v>
-      </c>
-      <c r="D19" s="3">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0</v>
-      </c>
-      <c r="G19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="3">
-        <v>3</v>
-      </c>
-      <c r="C20" s="3">
-        <v>2</v>
-      </c>
-      <c r="D20" s="3">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0</v>
-      </c>
-      <c r="G20" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="3">
-        <v>5</v>
-      </c>
-      <c r="C21" s="3">
-        <v>2</v>
-      </c>
-      <c r="D21" s="3">
-        <v>2</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0</v>
-      </c>
-      <c r="G21" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="3">
-        <v>6</v>
-      </c>
-      <c r="C22" s="3">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3">
-        <v>2</v>
-      </c>
-      <c r="E22" s="3">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0</v>
-      </c>
-      <c r="G22" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0</v>
-      </c>
-      <c r="G23" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="3">
-        <v>0</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3">
-        <v>2</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0</v>
-      </c>
-      <c r="G24" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="5">
-        <v>2</v>
-      </c>
-      <c r="C25" s="5">
-        <v>1</v>
-      </c>
-      <c r="D25" s="5">
-        <v>2</v>
-      </c>
-      <c r="E25" s="5">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5">
-        <v>0</v>
-      </c>
-      <c r="G25" s="6">
-        <v>1</v>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>